<commit_message>
modids wireframes et product backlog
</commit_message>
<xml_diff>
--- a/back/product backlog chexkpoint4.xlsx
+++ b/back/product backlog chexkpoint4.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="31">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -106,7 +106,10 @@
     <t xml:space="preserve">Accéder a la partie administratif du site</t>
   </si>
   <si>
-    <t xml:space="preserve">Gérer les changements du site</t>
+    <t xml:space="preserve">Gérer les changements du site autrement dit rajouter un projet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">en cours de développemnt</t>
   </si>
   <si>
     <t xml:space="preserve">                formulaire</t>
@@ -344,7 +347,7 @@
   <dimension ref="A1:Y11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -352,7 +355,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="26.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="26.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.57"/>
@@ -679,12 +682,14 @@
       <c r="E10" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="3"/>
+      <c r="F10" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="G10" s="3" t="n">
         <v>50</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>